<commit_message>
Component Selection and Antenna Design
Updated the component selection document to include more components, and some reasoning.

Wideband antenna designs were added to the schematic design document to facilitate the large bandwidth required by the pulsed waveform.

Pmax calculation was aded to the pulse radar calculation spreadsheet page.
</commit_message>
<xml_diff>
--- a/Electrical/Analysis+Design/RadarCalculators.xlsx
+++ b/Electrical/Analysis+Design/RadarCalculators.xlsx
@@ -16,6 +16,7 @@
     <sheet name="LinkBudget" sheetId="2" r:id="rId2"/>
     <sheet name="PulseRadar" sheetId="3" r:id="rId3"/>
     <sheet name="FMCWRadar" sheetId="4" r:id="rId4"/>
+    <sheet name="RCS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>Pt</t>
   </si>
@@ -210,6 +211,51 @@
   </si>
   <si>
     <t>SNR (dB)</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>Rmin</t>
+  </si>
+  <si>
+    <t>Tp</t>
+  </si>
+  <si>
+    <t>Ts</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Lpath</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Cabin Cruiser</t>
+  </si>
+  <si>
+    <t>Automobile</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>Corner Reflector</t>
+  </si>
+  <si>
+    <t>Missile</t>
+  </si>
+  <si>
+    <t>Stealth Aircraft</t>
   </si>
 </sst>
 </file>
@@ -280,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -288,12 +334,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -311,6 +372,18 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -601,291 +674,300 @@
   <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18.75">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="E2" s="13" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="E2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="14">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="19">
         <f>POWER(10, ($B$5 - 30)/10)</f>
         <v>0.1</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="19">
         <f>POWER($F$5*POWER($F$10*$F$11/1000, 2)*$B$10/(POWER(4*PI(),3)*$F$9), 0.25)</f>
-        <v>56.026251905705593</v>
-      </c>
-      <c r="K5" s="2" t="s">
+        <v>140.89856417214261</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
-        <v>200</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="18">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="19">
         <f>10*LOG10($B$17*($B$11+$B$19)*$B$6)+30+60</f>
-        <v>-90.917969741249408</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>-96.938569654528976</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="19">
+        <f>$F$6</f>
+        <v>-96.938569654528976</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="18">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="20">
         <f>POWER(10, ($F$6-30)/10)</f>
-        <v>8.094742272759921E-13</v>
-      </c>
-      <c r="G7" s="2" t="s">
+        <v>2.0236855681900015E-13</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="3"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="18">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="19">
         <f>$F$6+$B$7</f>
-        <v>-90.917969741249408</v>
-      </c>
-      <c r="G8" s="2" t="s">
+        <v>-96.938569654528976</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="3"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="18">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="20">
         <f>POWER(10, ($F$8-30)/10)</f>
-        <v>8.094742272759921E-13</v>
-      </c>
-      <c r="G9" s="2" t="s">
+        <v>2.0236855681900015E-13</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="3"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="18">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="19">
         <f>POWER(10, $B$8/10)</f>
         <v>3.9810717055349727</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="18">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="19">
         <f>$B$18/($B$9*1000000)</f>
         <v>99.930819333333332</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="14" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="18.75">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="20">
         <v>1.3806485199999999E-23</v>
       </c>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="18">
         <v>299792458</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="19">
         <v>273.14999999999998</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1620,12 +1702,399 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="5" max="7" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75">
+      <c r="A2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="19">
+        <f>POWER(10, ($B$5 - 30)/10)</f>
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="19">
+        <f>$B$18*($B$7+$B$8)*0.000000001/2</f>
+        <v>4.49688687</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="19">
+        <f>POWER(10, $B$9/10)</f>
+        <v>3.9810717055349727</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="19">
+        <f>-20*LOG10(POWER($F$6,2)*$B$11*POWER($F$7/1000,2)/(POWER(4*PI(),3)*POWER($J$5,4)))</f>
+        <v>94.197570871683865</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="18">
+        <f>1000/$B$6</f>
+        <v>20</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="19">
+        <f>$B$18/($B$10*1000000)</f>
+        <v>99.930819333333332</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="19">
+        <f>$B$5-$J$6</f>
+        <v>-74.197570871683865</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="15">
+        <v>10</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="18">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="18">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18">
+        <v>100</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75">
+      <c r="A14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1.3806485199999999E-23</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <v>299792458</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A14:C14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1635,7 +2104,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1646,4 +2115,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="16">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="16">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="16">
+        <v>100</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="16">
+        <v>20000</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>